<commit_message>
Start redesign of ADC board
</commit_message>
<xml_diff>
--- a/Sch/fm_bpf/fm_bpf.xlsx
+++ b/Sch/fm_bpf/fm_bpf.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="10056"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9912"/>
   </bookViews>
   <sheets>
     <sheet name="fm_bpf" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="136">
   <si>
     <t>Reference</t>
   </si>
@@ -480,6 +480,34 @@
   </si>
   <si>
     <t>Edge Connector</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Compatible parts can be used?</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Y</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -1137,7 +1165,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1154,6 +1182,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1478,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1493,10 +1524,11 @@
     <col min="6" max="6" width="25.44140625" customWidth="1"/>
     <col min="7" max="7" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1522,10 +1554,13 @@
         <v>42</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -1549,10 +1584,13 @@
         <v>63</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1575,9 +1613,12 @@
       <c r="H3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1602,9 +1643,12 @@
       <c r="H4" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -1629,9 +1673,12 @@
       <c r="H5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -1656,9 +1703,12 @@
       <c r="H6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1683,9 +1733,12 @@
       <c r="H7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -1710,9 +1763,12 @@
       <c r="H8" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1737,9 +1793,12 @@
       <c r="H9" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>71</v>
       </c>
@@ -1764,9 +1823,12 @@
       <c r="H10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1791,9 +1853,12 @@
       <c r="H11" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
@@ -1818,9 +1883,12 @@
       <c r="H12" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>90</v>
       </c>
@@ -1845,9 +1913,12 @@
       <c r="H13" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>18</v>
       </c>
@@ -1872,9 +1943,12 @@
       <c r="H14" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -1899,9 +1973,12 @@
       <c r="H15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I15" s="3"/>
+      <c r="I15" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
@@ -1926,9 +2003,12 @@
       <c r="H16" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I16" s="3"/>
+      <c r="I16" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
@@ -1953,9 +2033,12 @@
       <c r="H17" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -1980,9 +2063,12 @@
       <c r="H18" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="I18" s="3"/>
+      <c r="I18" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -2007,9 +2093,12 @@
       <c r="H19" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="I19" s="3"/>
+      <c r="I19" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>46</v>
       </c>
@@ -2034,9 +2123,12 @@
       <c r="H20" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="I20" s="3"/>
+      <c r="I20" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -2061,9 +2153,12 @@
       <c r="H21" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>37</v>
       </c>
@@ -2088,7 +2183,10 @@
       <c r="H22" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="I22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="J22" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>

</xml_diff>

<commit_message>
Fixed BOM for FM BPF
</commit_message>
<xml_diff>
--- a/Sch/fm_bpf/fm_bpf.xlsx
+++ b/Sch/fm_bpf/fm_bpf.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9912"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21264" windowHeight="8484"/>
   </bookViews>
   <sheets>
     <sheet name="fm_bpf" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="144">
   <si>
     <t>Reference</t>
   </si>
@@ -505,6 +505,34 @@
   <si>
     <t>Y</t>
     <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>W1,W2</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>TEST_1P</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>PTH</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>http://portal.fciconnect.com/Comergent//fci/drawing/68000.pdf</t>
+  </si>
+  <si>
+    <t>68000-401HLF</t>
+  </si>
+  <si>
+    <t>Amphenol FCI</t>
+  </si>
+  <si>
+    <t>BERGSTIK II .100" SR STRAIGHT</t>
   </si>
   <si>
     <t>Y</t>
@@ -515,7 +543,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -693,6 +721,14 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1165,7 +1201,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1185,6 +1221,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1509,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2188,6 +2236,34 @@
       </c>
       <c r="J22" s="3"/>
     </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J23" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18"/>
   <hyperlinks>

</xml_diff>